<commit_message>
calorimetry : tests : regression tests : save
</commit_message>
<xml_diff>
--- a/output/calorimetry/ds.3.ampoule.bad.no.opt/data.xlsx
+++ b/output/calorimetry/ds.3.ampoule.bad.no.opt/data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">H</t>
   </si>
@@ -111,82 +111,76 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
+    <t xml:space="preserve">tot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01911</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1e-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01486</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.004205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01451</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.004172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.004173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.004191</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.002568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.003495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.004183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.003492</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.004171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.003494</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.004179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.004182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lg_k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calorimeter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ampoule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">initial volume</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.01911</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1e-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.01486</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.01965</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.004205</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.01451</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.004172</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.004173</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.004191</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.002568</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.003495</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.004183</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.003492</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.004171</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.003494</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.004179</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.004182</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lg_k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calorimeter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ampoule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">component</t>
-  </si>
-  <si>
-    <t xml:space="preserve">initial volume</t>
   </si>
 </sst>
 </file>
@@ -987,15 +981,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1003,10 +997,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1474,98 +1468,98 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
+      <c r="A7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -1587,13 +1581,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
@@ -1609,178 +1603,178 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
         <v>36</v>
       </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1799,7 +1793,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
calorimetry : tests : regression tests
</commit_message>
<xml_diff>
--- a/output/calorimetry/ds.3.ampoule.bad.no.opt/data.xlsx
+++ b/output/calorimetry/ds.3.ampoule.bad.no.opt/data.xlsx
@@ -8,15 +8,14 @@
   <sheets>
     <sheet name="equilibrium_concentrations" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="heats_calculated" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="correlation_matrix" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="enthalpies_calculated" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="adj_r_squared" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="input_stoich_coefficients" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="input_concentrations" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="input_k_constants_log10" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="input_heats" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="input_enthalpies" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="setup" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="enthalpies_calculated" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="adj_r_squared" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="input_stoich_coefficients" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="input_concentrations" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="input_k_constants_log10" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="input_heats" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="input_enthalpies" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="setup" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
 </workbook>
 </file>
@@ -919,68 +918,6 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>-5.18</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>-2.96</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
         <v>48</v>
       </c>
       <c r="B1" t="s">
@@ -1318,7 +1255,96 @@
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-5.18</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>-2.96</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>9.47878966930947</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.197119914662341</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>11.2246759055297</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.25140680305007</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -1333,91 +1359,8 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>-5.18</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>-2.96</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>9.47878966930947</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.197119914662341</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>11.2246759055297</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.25140680305007</v>
+      <c r="A1" t="n">
+        <v>0.663618471219521</v>
       </c>
     </row>
   </sheetData>
@@ -1435,8 +1378,115 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
-        <v>0.663618471219521</v>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1455,114 +1505,200 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>0</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1581,200 +1717,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
+      <c r="A2" t="n">
+        <v>5.35</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
+      <c r="A3" t="n">
+        <v>7.34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
+      <c r="A4" t="n">
+        <v>7.44</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
+      <c r="A5" t="n">
+        <v>9.47</v>
       </c>
     </row>
   </sheetData>
@@ -1793,27 +1756,209 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5.35</v>
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>-10.0952</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-10.0952</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>7.34</v>
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-10.4137</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-10.4137</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>7.44</v>
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>-10.8359</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-10.8359</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>9.47</v>
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-10.7336</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-10.7336</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>-9.776</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-9.776</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-9.9857</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-9.9857</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-9.7711</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-9.7711</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-9.8545</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-9.8545</v>
       </c>
     </row>
   </sheetData>
@@ -1832,209 +1977,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-10.0952</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>-10.0952</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
-        <v>-10.4137</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
-        <v>-10.4137</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
-        <v>-10.8359</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="n">
-        <v>-10.8359</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
+      <c r="B5" t="n">
+        <v>-5.18</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
-        <v>-10.7336</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" t="n">
-        <v>-10.7336</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
       <c r="B6" t="n">
-        <v>-9.776</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>-9.776</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>-9.9857</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-9.9857</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>-9.7711</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" t="n">
-        <v>-9.7711</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>-9.8545</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" t="n">
-        <v>-9.8545</v>
+        <v>-2.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>